<commit_message>
calibration changes/testing final data
</commit_message>
<xml_diff>
--- a/TestingData.xlsx
+++ b/TestingData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Trial</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>FEV (measured)</t>
+  </si>
+  <si>
+    <t>FEV % Error</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,9 +381,11 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,204 +398,264 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3.0929000000000002</v>
+        <v>2.9658000000000002</v>
       </c>
       <c r="C2">
         <f>ABS(B2-3)/3*100</f>
-        <v>3.0966666666666738</v>
-      </c>
-      <c r="F2">
+        <v>1.139999999999993</v>
+      </c>
+      <c r="D2">
+        <v>2.5562999999999998</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <f>ABS(3-G2)/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5348999999999999</v>
+      </c>
+      <c r="I2">
+        <f>ABS(1.5-H2)/1.5*100</f>
+        <v>2.3266666666666618</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.6394000000000002</v>
+        <v>2.9298999999999999</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C11" si="0">ABS(B3-3)/3*100</f>
-        <v>12.019999999999992</v>
-      </c>
-      <c r="F3">
+        <v>2.3366666666666687</v>
+      </c>
+      <c r="D3">
+        <v>2.1509</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H11" si="1">ABS(3-G3)/3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5204</v>
+      </c>
+      <c r="I3">
+        <f>ABS(1.5-H3)/1.5*100</f>
+        <v>1.3599999999999981</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3.0516000000000001</v>
+        <v>2.9908000000000001</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>1.7200000000000031</v>
-      </c>
-      <c r="F4">
+        <v>0.30666666666666254</v>
+      </c>
+      <c r="D4">
+        <v>2.0684</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="I4">
+        <f>ABS(1.5-H4)/1.5*100</f>
+        <v>0.73333333333332651</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3.0144000000000002</v>
+        <v>3.0436999999999999</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.48000000000000637</v>
-      </c>
-      <c r="F5">
+        <v>1.4566666666666617</v>
+      </c>
+      <c r="D5">
+        <v>2.2814000000000001</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5168999999999999</v>
+      </c>
+      <c r="I5">
+        <f>ABS(1.5-H5)/1.5*100</f>
+        <v>1.1266666666666612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.0771999999999999</v>
+        <v>2.9897</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>2.5733333333333315</v>
-      </c>
-      <c r="F6">
+        <v>0.34333333333333249</v>
+      </c>
+      <c r="D6">
+        <v>1.7674000000000001</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5091000000000001</v>
+      </c>
+      <c r="I6">
+        <f>ABS(1.5-H6)/1.5*100</f>
+        <v>0.60666666666667379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3.0322</v>
+        <v>3.004</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.0733333333333337</v>
-      </c>
-      <c r="F7">
+        <v>0.13333333333333347</v>
+      </c>
+      <c r="D7">
+        <v>1.9328000000000001</v>
+      </c>
+      <c r="G7">
         <v>6</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5362</v>
+      </c>
+      <c r="I7">
+        <f>ABS(1.5-H7)/1.5*100</f>
+        <v>2.413333333333334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3.0426000000000002</v>
+        <v>3.0196000000000001</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.4200000000000066</v>
-      </c>
-      <c r="F8">
+        <v>0.65333333333333532</v>
+      </c>
+      <c r="D8">
+        <v>2.1667000000000001</v>
+      </c>
+      <c r="G8">
         <v>7</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5208999999999999</v>
+      </c>
+      <c r="I8">
+        <f>ABS(1.5-H8)/1.5*100</f>
+        <v>1.3933333333333278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3.0661999999999998</v>
+        <v>2.8353000000000002</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>2.2066666666666608</v>
-      </c>
-      <c r="F9">
+        <v>5.4899999999999949</v>
+      </c>
+      <c r="D9">
+        <v>2.5405000000000002</v>
+      </c>
+      <c r="G9">
         <v>8</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.4976</v>
+      </c>
+      <c r="I9">
+        <f>ABS(1.5-H9)/1.5*100</f>
+        <v>0.1599999999999972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3.0381</v>
+        <v>3.0272999999999999</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.2700000000000009</v>
-      </c>
-      <c r="F10">
+        <v>0.90999999999999603</v>
+      </c>
+      <c r="D10">
+        <v>2.1536</v>
+      </c>
+      <c r="G10">
         <v>9</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5338000000000001</v>
+      </c>
+      <c r="I10">
+        <f>ABS(1.5-H10)/1.5*100</f>
+        <v>2.2533333333333365</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3.0021</v>
+        <v>3.0329999999999999</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>6.9999999999999701E-2</v>
-      </c>
-      <c r="F11">
+        <v>1.0999999999999974</v>
+      </c>
+      <c r="D11">
+        <v>2.0937000000000001</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5072000000000001</v>
+      </c>
+      <c r="I11">
+        <f>ABS(1.5-H11)/1.5*100</f>
+        <v>0.48000000000000637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>